<commit_message>
hoàn thành chức năng xem báo cáo của sinh viên
</commit_message>
<xml_diff>
--- a/data/danhgiasinhvien/6.xlsx
+++ b/data/danhgiasinhvien/6.xlsx
@@ -22,7 +22,7 @@
     <x:t>name</x:t>
   </x:si>
   <x:si>
-    <x:t>commentOfLecture</x:t>
+    <x:t>comment</x:t>
   </x:si>
   <x:si>
     <x:t>Mark</x:t>
@@ -34,7 +34,7 @@
     <x:t>Con thủy quái</x:t>
   </x:si>
   <x:si>
-    <x:t>header</x:t>
+    <x:t>đẹp trai</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -430,7 +430,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="D3" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>